<commit_message>
Change to single data request and components revert back to store with static data
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="158">
   <si>
     <t>1. Static html page with Ext.onReady app</t>
   </si>
@@ -646,13 +646,19 @@
     <t>5. Getting data for multiple components from the server in one request</t>
   </si>
   <si>
-    <t>have 2 data requests</t>
-  </si>
-  <si>
     <t>Change to single data request and components revert back to arraystore with static data</t>
   </si>
   <si>
     <t>Add 2nd component (a line chart) using serverside data</t>
+  </si>
+  <si>
+    <t>NOTE we now have two independent AJAX requests on load to acquire data for the 2 components</t>
+  </si>
+  <si>
+    <t>2nd intiated by App1.store.SimpleChartStore.proxy</t>
+  </si>
+  <si>
+    <t>1st intiated by App1.store.SimpleStore.proxy</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V161"/>
+  <dimension ref="A1:V159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,229 +1625,239 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>151</v>
+      </c>
+    </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-      <c r="M119" s="2"/>
-      <c r="N119" s="2"/>
-      <c r="O119" s="2"/>
-      <c r="P119" s="2"/>
+      <c r="B119" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>151</v>
+      <c r="C120" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>116</v>
+      <c r="C121" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
-        <v>118</v>
+      <c r="D123" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>119</v>
+      <c r="D124" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
-        <v>120</v>
+      <c r="B125" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
-        <v>121</v>
+      <c r="C126" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C128" t="s">
-        <v>122</v>
+      <c r="C127" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A129" t="s">
         <v>146</v>
       </c>
     </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>124</v>
+      <c r="A132" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>125</v>
+      <c r="C134" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C136" t="s">
-        <v>126</v>
+      <c r="C135" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C137" t="s">
-        <v>127</v>
+      <c r="C137" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C139" s="1" t="s">
-        <v>128</v>
+      <c r="D139" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C140" t="s">
-        <v>129</v>
+      <c r="D140" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D142" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D143" t="s">
-        <v>132</v>
+      <c r="B143" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>148</v>
+      <c r="C145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C146" t="s">
-        <v>133</v>
-      </c>
+      <c r="C146" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C147" t="s">
-        <v>13</v>
-      </c>
       <c r="D147" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C148" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
+      <c r="E148" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D151" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E152" t="s">
-        <v>139</v>
+      <c r="B152" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
-        <v>149</v>
+      <c r="C154" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C157" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C158" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
+      <c r="B158" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" t="s">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1857,7 +1873,7 @@
     <hyperlink ref="U60" r:id="rId8" location="!/api/Ext.app.Application" display="http://docs.sencha.com/extjs/4.2.1/ - !/api/Ext.app.Application"/>
     <hyperlink ref="D73" r:id="rId9" location="!/api/Ext.app.Application" display="http://docs.sencha.com/extjs/4.2.1/ - !/api/Ext.app.Application"/>
     <hyperlink ref="D74" r:id="rId10" location="!/api/Ext.Loader" display="http://docs.sencha.com/extjs/4.2.1/ - !/api/Ext.Loader"/>
-    <hyperlink ref="C139" r:id="rId11"/>
+    <hyperlink ref="C137" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>